<commit_message>
Cleared all errors, also 25 students and 10 answer keys are displaying correctly
</commit_message>
<xml_diff>
--- a/CAT-Exam-Evaluation-System/dataset/data.xlsx
+++ b/CAT-Exam-Evaluation-System/dataset/data.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{489F789D-0783-4012-9497-D8302DC92AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CAT-Exam-Evaluation-System\CAT-Exam-Evaluation-System\dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE7CF6-5BD6-4570-9D3D-DFFE06BAAA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4580" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
-    <sheet name="Answers " sheetId="2" r:id="rId2"/>
+    <sheet name="Answers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L7"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="m6poU5cTb7qGxz55VXqt0lz7iiKGEkb/2FSc+hwEhZ8="/>
@@ -395,9 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView zoomScale="74" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1603,7 +1605,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Getting key answers from the excel file and converting it into a string
</commit_message>
<xml_diff>
--- a/CAT-Exam-Evaluation-System/dataset/data.xlsx
+++ b/CAT-Exam-Evaluation-System/dataset/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CAT-Exam-Evaluation-System\CAT-Exam-Evaluation-System\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE7CF6-5BD6-4570-9D3D-DFFE06BAAA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9C6DFA-0307-43C3-84CB-EC53F1CB2E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,10 +121,10 @@
     <t>c</t>
   </si>
   <si>
-    <t xml:space="preserve">Key Answers </t>
-  </si>
-  <si>
     <t>Sl No</t>
+  </si>
+  <si>
+    <t>Key Answers</t>
   </si>
 </sst>
 </file>
@@ -180,8 +180,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,7 +1605,9 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1613,11 +1615,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">

</xml_diff>